<commit_message>
Updated flow and operating expense calculation
</commit_message>
<xml_diff>
--- a/documentation/Pricing/OperatingExpenseCalculations.xlsx
+++ b/documentation/Pricing/OperatingExpenseCalculations.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,9 +32,6 @@
     <t>Units Subscribed</t>
   </si>
   <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>offer price</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>ContributorFactor</t>
+  </si>
+  <si>
+    <t>SnsitivityParamt</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="E2:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -418,7 +418,7 @@
   <sheetData>
     <row r="2" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1">
         <v>20000</v>
@@ -429,33 +429,33 @@
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
         <v>20</v>
@@ -464,7 +464,7 @@
         <v>22000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
@@ -475,23 +475,23 @@
       </c>
       <c r="K5" s="1">
         <f>$F$2/$J$10</f>
-        <v>2.5940337224383916E-3</v>
+        <v>3.5304501323918801E-3</v>
       </c>
       <c r="L5" s="1">
         <v>22000</v>
       </c>
       <c r="M5" s="1">
         <f>K5*F5*I5</f>
-        <v>5.188067444876783E-2</v>
+        <v>7.0609002647837607E-2</v>
       </c>
       <c r="N5" s="1">
         <f>G5*M5</f>
-        <v>1141.3748378728922</v>
+        <v>1553.3980582524273</v>
       </c>
     </row>
     <row r="6" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
         <v>40</v>
@@ -500,7 +500,7 @@
         <v>34000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I6" s="1">
         <v>1</v>
@@ -511,23 +511,23 @@
       </c>
       <c r="K6" s="1">
         <f t="shared" ref="K6:K9" si="1">$F$2/$J$10</f>
-        <v>2.5940337224383916E-3</v>
+        <v>3.5304501323918801E-3</v>
       </c>
       <c r="L6" s="1">
         <v>34000</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" ref="M6:M8" si="2">K6*F6*I6</f>
-        <v>0.10376134889753566</v>
+        <v>0.14121800529567521</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6:N9" si="3">G6*M6</f>
-        <v>3527.8858625162125</v>
+        <v>4801.4121800529574</v>
       </c>
     </row>
     <row r="7" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1">
         <v>50</v>
@@ -536,7 +536,7 @@
         <v>38000</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I7" s="1">
         <v>1.2</v>
@@ -547,59 +547,59 @@
       </c>
       <c r="K7" s="1">
         <f t="shared" si="1"/>
-        <v>2.5940337224383916E-3</v>
+        <v>3.5304501323918801E-3</v>
       </c>
       <c r="L7" s="1">
         <v>45600</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" si="2"/>
-        <v>0.15564202334630348</v>
+        <v>0.21182700794351281</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="3"/>
-        <v>5914.3968871595325</v>
+        <v>8049.4263018534866</v>
       </c>
     </row>
     <row r="8" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>50</v>
       </c>
       <c r="G8" s="1">
-        <v>41000</v>
+        <v>100</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I8" s="1">
         <v>1.2</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="0"/>
-        <v>2050000</v>
+        <v>5000</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>2.5940337224383916E-3</v>
+        <v>3.5304501323918801E-3</v>
       </c>
       <c r="L8" s="1">
         <v>49200</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" si="2"/>
-        <v>0.15564202334630348</v>
+        <v>0.21182700794351281</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="3"/>
-        <v>6381.322957198443</v>
+        <v>21.18270079435128</v>
       </c>
     </row>
     <row r="9" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="1">
         <v>70</v>
@@ -608,7 +608,7 @@
         <v>28000</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I9" s="1">
         <v>1</v>
@@ -619,27 +619,27 @@
       </c>
       <c r="K9" s="1">
         <f t="shared" si="1"/>
-        <v>2.5940337224383916E-3</v>
+        <v>3.5304501323918801E-3</v>
       </c>
       <c r="L9" s="1">
         <v>28000</v>
       </c>
       <c r="M9" s="1">
         <f>K9*F9*I9</f>
-        <v>0.18158236057068741</v>
+        <v>0.2471315092674316</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>5084.3060959792474</v>
+        <v>6919.682259488085</v>
       </c>
     </row>
     <row r="10" spans="5:14" x14ac:dyDescent="0.35">
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" s="1">
         <f>SUM(J5:J9)</f>
-        <v>7710000</v>
+        <v>5665000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>